<commit_message>
ID -> id 통일
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -481,263 +481,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-05-24 23:26:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-05-24 23:26:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-05-24 23:58:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-05-25 00:41:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-05-25 01:03:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-05-25 01:03:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-05-25 01:04:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-05-25 01:30:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>yeong nam</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1234567890</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2024-05-25 01:31:04</t>
+          <t>2024-05-25 18:28:31</t>
         </is>
       </c>
     </row>

</xml_diff>